<commit_message>
alle documenten samen aan hetvoegen
nog niet klaar
</commit_message>
<xml_diff>
--- a/documents/@Planner/Planner biocodegaming.xlsx
+++ b/documents/@Planner/Planner biocodegaming.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\damia\Dropbox\@USBWebserver v8.6\root\A_PROFTAAK-WEB\Proftaak-biocodegaming-web\documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexm\Desktop\USBWEB\root\Proftaak-biocodegaming-web\documents\@Planner\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="12576"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Projects Overview" sheetId="1" r:id="rId1"/>
@@ -568,7 +568,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="d/m/yyyy"/>
+      <numFmt numFmtId="165" formatCode="d/m/yyyy"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -651,298 +651,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>1085851</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>205740</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>3185161</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>542926</xdr:rowOff>
-    </xdr:to>
-    <xdr:grpSp>
-      <xdr:nvGrpSpPr>
-        <xdr:cNvPr id="4" name="Task Details" descr="Click this shape to switch to the Task Details tab." title="Navigation Button - Task Detail">
-          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" tooltip="Click to view Task Details sheet."/>
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGrpSpPr/>
-      </xdr:nvGrpSpPr>
-      <xdr:grpSpPr>
-        <a:xfrm>
-          <a:off x="7738111" y="205740"/>
-          <a:ext cx="2099310" cy="337186"/>
-          <a:chOff x="2933700" y="6505574"/>
-          <a:chExt cx="2476500" cy="342901"/>
-        </a:xfrm>
-      </xdr:grpSpPr>
-      <xdr:sp macro="[0]!Sheet1.ShowTasks" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="5" name="Freeform 6">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr>
-            <a:spLocks/>
-          </xdr:cNvSpPr>
-        </xdr:nvSpPr>
-        <xdr:spPr bwMode="auto">
-          <a:xfrm>
-            <a:off x="5286375" y="6638925"/>
-            <a:ext cx="66675" cy="133350"/>
-          </a:xfrm>
-          <a:custGeom>
-            <a:avLst/>
-            <a:gdLst>
-              <a:gd name="T0" fmla="*/ 0 w 1633"/>
-              <a:gd name="T1" fmla="*/ 0 h 3029"/>
-              <a:gd name="T2" fmla="*/ 759 w 1633"/>
-              <a:gd name="T3" fmla="*/ 0 h 3029"/>
-              <a:gd name="T4" fmla="*/ 1633 w 1633"/>
-              <a:gd name="T5" fmla="*/ 1514 h 3029"/>
-              <a:gd name="T6" fmla="*/ 759 w 1633"/>
-              <a:gd name="T7" fmla="*/ 3029 h 3029"/>
-              <a:gd name="T8" fmla="*/ 5 w 1633"/>
-              <a:gd name="T9" fmla="*/ 3029 h 3029"/>
-              <a:gd name="T10" fmla="*/ 884 w 1633"/>
-              <a:gd name="T11" fmla="*/ 1514 h 3029"/>
-              <a:gd name="T12" fmla="*/ 0 w 1633"/>
-              <a:gd name="T13" fmla="*/ 0 h 3029"/>
-            </a:gdLst>
-            <a:ahLst/>
-            <a:cxnLst>
-              <a:cxn ang="0">
-                <a:pos x="T0" y="T1"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="T2" y="T3"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="T4" y="T5"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="T6" y="T7"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="T8" y="T9"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="T10" y="T11"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="T12" y="T13"/>
-              </a:cxn>
-            </a:cxnLst>
-            <a:rect l="0" t="0" r="r" b="b"/>
-            <a:pathLst>
-              <a:path w="1633" h="3029">
-                <a:moveTo>
-                  <a:pt x="0" y="0"/>
-                </a:moveTo>
-                <a:lnTo>
-                  <a:pt x="759" y="0"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="1633" y="1514"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="759" y="3029"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="5" y="3029"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="884" y="1514"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="0" y="0"/>
-                </a:lnTo>
-                <a:close/>
-              </a:path>
-            </a:pathLst>
-          </a:custGeom>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln w="0">
-            <a:noFill/>
-            <a:prstDash val="solid"/>
-            <a:round/>
-            <a:headEnd/>
-            <a:tailEnd/>
-          </a:ln>
-        </xdr:spPr>
-      </xdr:sp>
-      <xdr:sp macro="[0]!Sheet1.ShowTasks" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="6" name="Freeform 7">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr>
-            <a:spLocks/>
-          </xdr:cNvSpPr>
-        </xdr:nvSpPr>
-        <xdr:spPr bwMode="auto">
-          <a:xfrm>
-            <a:off x="5343525" y="6638925"/>
-            <a:ext cx="66675" cy="133350"/>
-          </a:xfrm>
-          <a:custGeom>
-            <a:avLst/>
-            <a:gdLst>
-              <a:gd name="T0" fmla="*/ 0 w 1633"/>
-              <a:gd name="T1" fmla="*/ 0 h 3029"/>
-              <a:gd name="T2" fmla="*/ 759 w 1633"/>
-              <a:gd name="T3" fmla="*/ 0 h 3029"/>
-              <a:gd name="T4" fmla="*/ 1633 w 1633"/>
-              <a:gd name="T5" fmla="*/ 1514 h 3029"/>
-              <a:gd name="T6" fmla="*/ 759 w 1633"/>
-              <a:gd name="T7" fmla="*/ 3029 h 3029"/>
-              <a:gd name="T8" fmla="*/ 5 w 1633"/>
-              <a:gd name="T9" fmla="*/ 3029 h 3029"/>
-              <a:gd name="T10" fmla="*/ 884 w 1633"/>
-              <a:gd name="T11" fmla="*/ 1514 h 3029"/>
-              <a:gd name="T12" fmla="*/ 0 w 1633"/>
-              <a:gd name="T13" fmla="*/ 0 h 3029"/>
-            </a:gdLst>
-            <a:ahLst/>
-            <a:cxnLst>
-              <a:cxn ang="0">
-                <a:pos x="T0" y="T1"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="T2" y="T3"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="T4" y="T5"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="T6" y="T7"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="T8" y="T9"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="T10" y="T11"/>
-              </a:cxn>
-              <a:cxn ang="0">
-                <a:pos x="T12" y="T13"/>
-              </a:cxn>
-            </a:cxnLst>
-            <a:rect l="0" t="0" r="r" b="b"/>
-            <a:pathLst>
-              <a:path w="1633" h="3029">
-                <a:moveTo>
-                  <a:pt x="0" y="0"/>
-                </a:moveTo>
-                <a:lnTo>
-                  <a:pt x="759" y="0"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="1633" y="1514"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="759" y="3029"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="5" y="3029"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="884" y="1514"/>
-                </a:lnTo>
-                <a:lnTo>
-                  <a:pt x="0" y="0"/>
-                </a:lnTo>
-                <a:close/>
-              </a:path>
-            </a:pathLst>
-          </a:custGeom>
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:ln w="0">
-            <a:noFill/>
-            <a:prstDash val="solid"/>
-            <a:round/>
-            <a:headEnd/>
-            <a:tailEnd/>
-          </a:ln>
-        </xdr:spPr>
-      </xdr:sp>
-      <xdr:sp macro="[0]!Sheet1.ShowTasks" textlink="">
-        <xdr:nvSpPr>
-          <xdr:cNvPr id="7" name="TextBox 6" title="Navigation Button Label - Task Detail">
-            <a:extLst>
-              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007000000}"/>
-              </a:ext>
-            </a:extLst>
-          </xdr:cNvPr>
-          <xdr:cNvSpPr txBox="1"/>
-        </xdr:nvSpPr>
-        <xdr:spPr>
-          <a:xfrm>
-            <a:off x="2933700" y="6505574"/>
-            <a:ext cx="1946141" cy="342901"/>
-          </a:xfrm>
-          <a:prstGeom prst="rect">
-            <a:avLst/>
-          </a:prstGeom>
-          <a:noFill/>
-          <a:ln w="9525" cmpd="sng">
-            <a:noFill/>
-          </a:ln>
-        </xdr:spPr>
-        <xdr:style>
-          <a:lnRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:lnRef>
-          <a:fillRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:fillRef>
-          <a:effectRef idx="0">
-            <a:scrgbClr r="0" g="0" b="0"/>
-          </a:effectRef>
-          <a:fontRef idx="minor">
-            <a:schemeClr val="dk1"/>
-          </a:fontRef>
-        </xdr:style>
-        <xdr:txBody>
-          <a:bodyPr vertOverflow="overflow" horzOverflow="overflow" wrap="none" rtlCol="0" anchor="b"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr algn="r"/>
-            <a:endParaRPr lang="en-US" sz="1400" b="1">
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:latin typeface="+mj-lt"/>
-              <a:cs typeface="DokChampa" pitchFamily="34" charset="-34"/>
-            </a:endParaRPr>
-          </a:p>
-        </xdr:txBody>
-      </xdr:sp>
-    </xdr:grpSp>
-    <xdr:clientData fPrintsWithSheet="0"/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
@@ -970,7 +678,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -2229,18 +1937,18 @@
   <dimension ref="B1:G31"/>
   <sheetViews>
     <sheetView showGridLines="0" showZeros="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.875" customWidth="1"/>
-    <col min="2" max="2" width="34.25" customWidth="1"/>
+    <col min="1" max="1" width="3.85546875" customWidth="1"/>
+    <col min="2" max="2" width="34.28515625" customWidth="1"/>
     <col min="3" max="3" width="71" customWidth="1"/>
-    <col min="4" max="4" width="28.875" hidden="1" customWidth="1"/>
-    <col min="5" max="6" width="14.25" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="61.25" customWidth="1"/>
-    <col min="8" max="8" width="3.875" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" hidden="1" customWidth="1"/>
+    <col min="5" max="6" width="14.28515625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="61.28515625" customWidth="1"/>
+    <col min="8" max="8" width="3.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2372,7 +2080,7 @@
       </c>
       <c r="G8" s="2"/>
     </row>
-    <row r="9" spans="2:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:7" ht="17.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="22">
         <v>42876</v>
       </c>
@@ -2835,13 +2543,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.875" customWidth="1"/>
+    <col min="1" max="1" width="3.85546875" customWidth="1"/>
     <col min="2" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="33" customWidth="1"/>
-    <col min="5" max="5" width="42.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.875" customWidth="1"/>
-    <col min="7" max="7" width="40.75" customWidth="1"/>
-    <col min="8" max="8" width="3.875" customWidth="1"/>
+    <col min="5" max="5" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" customWidth="1"/>
+    <col min="7" max="7" width="40.7109375" customWidth="1"/>
+    <col min="8" max="8" width="3.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
changed planner and began with reg
</commit_message>
<xml_diff>
--- a/documents/@Planner/Planner biocodegaming.xlsx
+++ b/documents/@Planner/Planner biocodegaming.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="69">
   <si>
     <t>Project</t>
   </si>
@@ -148,9 +148,6 @@
     <t>Plan Sara's Surprise Party</t>
   </si>
   <si>
-    <t xml:space="preserve"> days</t>
-  </si>
-  <si>
     <t>functioneel en technische ontwerp af maken.</t>
   </si>
   <si>
@@ -196,7 +193,89 @@
     <t>alex finished de documenten</t>
   </si>
   <si>
-    <t>groen = dag voorbij          geel = vrij/weekend</t>
+    <t>damian is begonnen met het register system, alex aan het forum</t>
+  </si>
+  <si>
+    <t>login bugged, moet nocker voor hulp vragen</t>
+  </si>
+  <si>
+    <t>day</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> date</t>
+  </si>
+  <si>
+    <t>MA</t>
+  </si>
+  <si>
+    <t>DI</t>
+  </si>
+  <si>
+    <t>WO</t>
+  </si>
+  <si>
+    <t>DO</t>
+  </si>
+  <si>
+    <t>VR</t>
+  </si>
+  <si>
+    <t>ZA</t>
+  </si>
+  <si>
+    <t>ZO</t>
+  </si>
+  <si>
+    <t>Di</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="9"/>
+        <color theme="8"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>groen</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = dag voorbij          </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="9"/>
+        <color rgb="FFF8F200"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>geel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1" tint="0.34998626667073579"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> = vrij/weekend</t>
+    </r>
+  </si>
+  <si>
+    <t>het uurt te lang ugh</t>
   </si>
 </sst>
 </file>
@@ -206,7 +285,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="9"/>
       <color theme="1" tint="0.34998626667073579"/>
@@ -299,6 +378,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="9"/>
+      <color theme="8"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="9"/>
+      <color rgb="FFF8F200"/>
+      <name val="Century Gothic"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -347,7 +451,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -362,8 +466,9 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -448,8 +553,14 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="6" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="8" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="9">
     <cellStyle name="Chart" xfId="4"/>
     <cellStyle name="Check Cell" xfId="6" builtinId="23"/>
     <cellStyle name="Good" xfId="7" builtinId="26"/>
@@ -458,6 +569,7 @@
     <cellStyle name="Neutral" xfId="5" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Title" xfId="8" builtinId="15"/>
   </cellStyles>
   <dxfs count="21">
     <dxf>
@@ -674,6 +786,11 @@
       <tableStyleElement type="firstColumn" dxfId="18"/>
     </tableStyle>
   </tableStyles>
+  <colors>
+    <mruColors>
+      <color rgb="FFF8F200"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -689,13 +806,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>274320</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>266700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>441960</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -739,13 +856,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>289560</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>457200</xdr:colOff>
       <xdr:row>24</xdr:row>
       <xdr:rowOff>205740</xdr:rowOff>
@@ -789,13 +906,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>14</xdr:col>
       <xdr:colOff>472440</xdr:colOff>
       <xdr:row>37</xdr:row>
       <xdr:rowOff>167640</xdr:rowOff>
@@ -1786,10 +1903,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Projects" displayName="Projects" ref="B3:G43" headerRowDxfId="17">
-  <autoFilter ref="B3:G43"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Projects" displayName="Projects" ref="C3:H43" headerRowDxfId="17">
+  <autoFilter ref="C3:H43"/>
   <tableColumns count="6">
-    <tableColumn id="4" name=" days" dataDxfId="16" totalsRowDxfId="15">
+    <tableColumn id="4" name=" date" dataDxfId="16" totalsRowDxfId="15">
       <calculatedColumnFormula array="1">MIN(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[Start]))</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="1" name="Project" totalsRowLabel="Total" totalsRowDxfId="14" dataCellStyle="Indent"/>
@@ -2070,859 +2187,1029 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:G43"/>
+  <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView showGridLines="0" showZeros="0" tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.875" customWidth="1"/>
-    <col min="2" max="2" width="34.25" customWidth="1"/>
-    <col min="3" max="3" width="71" customWidth="1"/>
-    <col min="4" max="4" width="28.875" hidden="1" customWidth="1"/>
-    <col min="5" max="6" width="14.25" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="61.25" customWidth="1"/>
-    <col min="8" max="8" width="3.875" customWidth="1"/>
+    <col min="2" max="2" width="3.875" customWidth="1"/>
+    <col min="3" max="3" width="34.25" customWidth="1"/>
+    <col min="4" max="4" width="71" customWidth="1"/>
+    <col min="5" max="5" width="28.875" hidden="1" customWidth="1"/>
+    <col min="6" max="7" width="14.25" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="61.25" customWidth="1"/>
+    <col min="9" max="9" width="3.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="25" t="s">
+    <row r="1" spans="1:8" ht="52.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:8" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="28"/>
+      <c r="C3" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="29"/>
+      <c r="C4" s="26">
+        <v>42871</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="5">
+        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
+        <v>1E-4</v>
+      </c>
+      <c r="F4" s="4" t="str">
+        <f>REPT("|",Projects[[  ]]*175)</f>
+        <v/>
+      </c>
+      <c r="G4" s="11">
+        <f t="array" ref="G4">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
+        <v>0</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="29"/>
+      <c r="C5" s="26">
+        <v>42872</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="5">
+        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
+        <v>1E-4</v>
+      </c>
+      <c r="F5" s="4" t="str">
+        <f>REPT("|",Projects[[  ]]*175)</f>
+        <v/>
+      </c>
+      <c r="G5" s="11">
+        <f t="array" ref="G5">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
+        <v>0</v>
+      </c>
+      <c r="H5" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G1" t="s">
+    </row>
+    <row r="6" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="29"/>
+      <c r="C6" s="26">
+        <v>42873</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="5">
+        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
+        <v>1E-4</v>
+      </c>
+      <c r="F6" s="4" t="str">
+        <f>REPT("|",Projects[[  ]]*175)</f>
+        <v/>
+      </c>
+      <c r="G6" s="11">
+        <f t="array" ref="G6">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="29"/>
+      <c r="C7" s="26">
+        <v>42874</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="6">
+        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
+        <v>1E-4</v>
+      </c>
+      <c r="F7" s="4" t="str">
+        <f>REPT("|",Projects[[  ]]*175)</f>
+        <v/>
+      </c>
+      <c r="G7" s="8">
+        <f t="array" ref="G7">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
+        <v>0</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8" s="29"/>
+      <c r="C8" s="22">
+        <v>42875</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="19">
+        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
+        <v>1E-4</v>
+      </c>
+      <c r="F8" s="20" t="str">
+        <f>REPT("|",Projects[[  ]]*175)</f>
+        <v/>
+      </c>
+      <c r="G8" s="17">
+        <f t="array" ref="G8">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
+        <v>0</v>
+      </c>
+      <c r="H8" s="27"/>
+    </row>
+    <row r="9" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" s="29"/>
+      <c r="C9" s="22">
+        <v>42876</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="19">
+        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
+        <v>1E-4</v>
+      </c>
+      <c r="F9" s="20" t="str">
+        <f>REPT("|",Projects[[  ]]*175)</f>
+        <v/>
+      </c>
+      <c r="G9" s="17">
+        <f t="array" ref="G9">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
+        <v>0</v>
+      </c>
+      <c r="H9" s="27"/>
+    </row>
+    <row r="10" spans="1:8" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" s="29"/>
+      <c r="C10" s="26">
+        <v>42877</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E10" s="19">
+        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
+        <v>1E-4</v>
+      </c>
+      <c r="F10" s="20" t="str">
+        <f>REPT("|",Projects[[  ]]*175)</f>
+        <v/>
+      </c>
+      <c r="G10" s="17">
+        <f t="array" ref="G10">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
+        <v>0</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="29"/>
+      <c r="C11" s="26">
+        <v>42878</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E11" s="19">
+        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
+        <v>1E-4</v>
+      </c>
+      <c r="F11" s="20" t="str">
+        <f>REPT("|",Projects[[  ]]*175)</f>
+        <v/>
+      </c>
+      <c r="G11" s="17">
+        <f t="array" ref="G11">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
+        <v>0</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="29"/>
+      <c r="C12" s="26">
+        <v>42879</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="19">
+        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
+        <v>1E-4</v>
+      </c>
+      <c r="F12" s="20" t="str">
+        <f>REPT("|",Projects[[  ]]*175)</f>
+        <v/>
+      </c>
+      <c r="G12" s="17">
+        <f t="array" ref="G12">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="2:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="2:7" ht="18" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="F3" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" s="23" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="26">
-        <v>42871</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D4" s="5">
-        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
-        <v>1E-4</v>
-      </c>
-      <c r="E4" s="4" t="str">
-        <f>REPT("|",Projects[[  ]]*175)</f>
-        <v/>
-      </c>
-      <c r="F4" s="11">
-        <f t="array" ref="F4">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
-        <v>0</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="26">
-        <v>42872</v>
-      </c>
-      <c r="C5" s="2" t="s">
+    <row r="13" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="29"/>
+      <c r="C13" s="22">
+        <v>42880</v>
+      </c>
+      <c r="D13" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="5">
-        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
-        <v>1E-4</v>
-      </c>
-      <c r="E5" s="4" t="str">
-        <f>REPT("|",Projects[[  ]]*175)</f>
-        <v/>
-      </c>
-      <c r="F5" s="11">
-        <f t="array" ref="F5">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
-        <v>0</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="26">
-        <v>42873</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="D6" s="5">
-        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
-        <v>1E-4</v>
-      </c>
-      <c r="E6" s="4" t="str">
-        <f>REPT("|",Projects[[  ]]*175)</f>
-        <v/>
-      </c>
-      <c r="F6" s="11">
-        <f t="array" ref="F6">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
-        <v>0</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="26">
-        <v>42874</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" s="6">
-        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
-        <v>1E-4</v>
-      </c>
-      <c r="E7" s="4" t="str">
-        <f>REPT("|",Projects[[  ]]*175)</f>
-        <v/>
-      </c>
-      <c r="F7" s="8">
-        <f t="array" ref="F7">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
-        <v>0</v>
-      </c>
-      <c r="G7" s="2"/>
-    </row>
-    <row r="8" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="22">
-        <v>42875</v>
-      </c>
-      <c r="C8" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="D8" s="19">
-        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
-        <v>1E-4</v>
-      </c>
-      <c r="E8" s="20" t="str">
-        <f>REPT("|",Projects[[  ]]*175)</f>
-        <v/>
-      </c>
-      <c r="F8" s="17">
-        <f t="array" ref="F8">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
-        <v>0</v>
-      </c>
-      <c r="G8" s="27"/>
-    </row>
-    <row r="9" spans="2:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="22">
-        <v>42876</v>
-      </c>
-      <c r="C9" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="D9" s="19">
-        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
-        <v>1E-4</v>
-      </c>
-      <c r="E9" s="20" t="str">
-        <f>REPT("|",Projects[[  ]]*175)</f>
-        <v/>
-      </c>
-      <c r="F9" s="17">
-        <f t="array" ref="F9">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
-        <v>0</v>
-      </c>
-      <c r="G9" s="27"/>
-    </row>
-    <row r="10" spans="2:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="26">
-        <v>42877</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D10" s="19">
-        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
-        <v>1E-4</v>
-      </c>
-      <c r="E10" s="20" t="str">
-        <f>REPT("|",Projects[[  ]]*175)</f>
-        <v/>
-      </c>
-      <c r="F10" s="17">
-        <f t="array" ref="F10">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
-        <v>0</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="26">
-        <v>42878</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D11" s="19">
-        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
-        <v>1E-4</v>
-      </c>
-      <c r="E11" s="20" t="str">
-        <f>REPT("|",Projects[[  ]]*175)</f>
-        <v/>
-      </c>
-      <c r="F11" s="17">
-        <f t="array" ref="F11">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
-        <v>0</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="18">
-        <v>42879</v>
-      </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="19">
-        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
-        <v>1E-4</v>
-      </c>
-      <c r="E12" s="20" t="str">
-        <f>REPT("|",Projects[[  ]]*175)</f>
-        <v/>
-      </c>
-      <c r="F12" s="17">
-        <f t="array" ref="F12">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
-        <v>0</v>
-      </c>
-      <c r="G12" s="2"/>
-    </row>
-    <row r="13" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="22">
-        <v>42880</v>
-      </c>
-      <c r="C13" s="27" t="s">
+      <c r="E13" s="19">
+        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
+        <v>1E-4</v>
+      </c>
+      <c r="F13" s="20" t="str">
+        <f>REPT("|",Projects[[  ]]*175)</f>
+        <v/>
+      </c>
+      <c r="G13" s="17">
+        <f t="array" ref="G13">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="27"/>
+    </row>
+    <row r="14" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="29"/>
+      <c r="C14" s="22">
+        <v>42881</v>
+      </c>
+      <c r="D14" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="19">
-        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
-        <v>1E-4</v>
-      </c>
-      <c r="E13" s="20" t="str">
-        <f>REPT("|",Projects[[  ]]*175)</f>
-        <v/>
-      </c>
-      <c r="F13" s="17">
-        <f t="array" ref="F13">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
-        <v>0</v>
-      </c>
-      <c r="G13" s="27"/>
-    </row>
-    <row r="14" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="22">
-        <v>42881</v>
-      </c>
-      <c r="C14" s="27" t="s">
+      <c r="E14" s="19">
+        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
+        <v>1E-4</v>
+      </c>
+      <c r="F14" s="20" t="str">
+        <f>REPT("|",Projects[[  ]]*175)</f>
+        <v/>
+      </c>
+      <c r="G14" s="17">
+        <f t="array" ref="G14">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
+        <v>0</v>
+      </c>
+      <c r="H14" s="27"/>
+    </row>
+    <row r="15" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="29"/>
+      <c r="C15" s="22">
+        <v>42882</v>
+      </c>
+      <c r="D15" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="19">
-        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
-        <v>1E-4</v>
-      </c>
-      <c r="E14" s="20" t="str">
-        <f>REPT("|",Projects[[  ]]*175)</f>
-        <v/>
-      </c>
-      <c r="F14" s="17">
-        <f t="array" ref="F14">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
-        <v>0</v>
-      </c>
-      <c r="G14" s="27"/>
-    </row>
-    <row r="15" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="22">
-        <v>42882</v>
-      </c>
-      <c r="C15" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" s="19">
-        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
-        <v>1E-4</v>
-      </c>
-      <c r="E15" s="20" t="str">
-        <f>REPT("|",Projects[[  ]]*175)</f>
-        <v/>
-      </c>
-      <c r="F15" s="17">
-        <f t="array" ref="F15">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
-        <v>0</v>
-      </c>
-      <c r="G15" s="27"/>
-    </row>
-    <row r="16" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="22">
+      <c r="E15" s="19">
+        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
+        <v>1E-4</v>
+      </c>
+      <c r="F15" s="20" t="str">
+        <f>REPT("|",Projects[[  ]]*175)</f>
+        <v/>
+      </c>
+      <c r="G15" s="17">
+        <f t="array" ref="G15">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
+        <v>0</v>
+      </c>
+      <c r="H15" s="27"/>
+    </row>
+    <row r="16" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="B16" s="29"/>
+      <c r="C16" s="22">
         <v>42883</v>
       </c>
-      <c r="C16" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" s="19">
-        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
-        <v>1E-4</v>
-      </c>
-      <c r="E16" s="20" t="str">
-        <f>REPT("|",Projects[[  ]]*175)</f>
-        <v/>
-      </c>
-      <c r="F16" s="17">
-        <f t="array" ref="F16">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
-        <v>0</v>
-      </c>
-      <c r="G16" s="27"/>
-    </row>
-    <row r="17" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="18">
+      <c r="D16" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="E16" s="19">
+        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
+        <v>1E-4</v>
+      </c>
+      <c r="F16" s="20" t="str">
+        <f>REPT("|",Projects[[  ]]*175)</f>
+        <v/>
+      </c>
+      <c r="G16" s="17">
+        <f t="array" ref="G16">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
+        <v>0</v>
+      </c>
+      <c r="H16" s="27"/>
+    </row>
+    <row r="17" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="29"/>
+      <c r="C17" s="18">
         <v>42884</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="21">
-        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
-        <v>1E-4</v>
-      </c>
-      <c r="E17" s="20" t="str">
-        <f>REPT("|",Projects[[  ]]*175)</f>
-        <v/>
-      </c>
-      <c r="F17" s="17">
-        <f t="array" ref="F17">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
-        <v>0</v>
-      </c>
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="18">
+      <c r="D17" s="2"/>
+      <c r="E17" s="21">
+        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
+        <v>1E-4</v>
+      </c>
+      <c r="F17" s="20" t="str">
+        <f>REPT("|",Projects[[  ]]*175)</f>
+        <v/>
+      </c>
+      <c r="G17" s="17">
+        <f t="array" ref="G17">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
+        <v>0</v>
+      </c>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B18" s="29"/>
+      <c r="C18" s="18">
         <v>42885</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="21">
-        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
-        <v>1E-4</v>
-      </c>
-      <c r="E18" s="20" t="str">
-        <f>REPT("|",Projects[[  ]]*175)</f>
-        <v/>
-      </c>
-      <c r="F18" s="17">
-        <f t="array" ref="F18">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
-        <v>0</v>
-      </c>
-      <c r="G18" s="2"/>
-    </row>
-    <row r="19" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="18">
+      <c r="D18" s="2"/>
+      <c r="E18" s="21">
+        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
+        <v>1E-4</v>
+      </c>
+      <c r="F18" s="20" t="str">
+        <f>REPT("|",Projects[[  ]]*175)</f>
+        <v/>
+      </c>
+      <c r="G18" s="17">
+        <f t="array" ref="G18">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
+        <v>0</v>
+      </c>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="B19" s="29"/>
+      <c r="C19" s="18">
         <v>42886</v>
       </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="21">
-        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
-        <v>1E-4</v>
-      </c>
-      <c r="E19" s="20" t="str">
-        <f>REPT("|",Projects[[  ]]*175)</f>
-        <v/>
-      </c>
-      <c r="F19" s="17">
-        <f t="array" ref="F19">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
-        <v>0</v>
-      </c>
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="18">
+      <c r="D19" s="2"/>
+      <c r="E19" s="21">
+        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
+        <v>1E-4</v>
+      </c>
+      <c r="F19" s="20" t="str">
+        <f>REPT("|",Projects[[  ]]*175)</f>
+        <v/>
+      </c>
+      <c r="G19" s="17">
+        <f t="array" ref="G19">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
+        <v>0</v>
+      </c>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="29"/>
+      <c r="C20" s="18">
         <v>42887</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="21">
-        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
-        <v>1E-4</v>
-      </c>
-      <c r="E20" s="20" t="str">
-        <f>REPT("|",Projects[[  ]]*175)</f>
-        <v/>
-      </c>
-      <c r="F20" s="17">
-        <f t="array" ref="F20">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
-        <v>0</v>
-      </c>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="18">
+      <c r="D20" s="2"/>
+      <c r="E20" s="21">
+        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
+        <v>1E-4</v>
+      </c>
+      <c r="F20" s="20" t="str">
+        <f>REPT("|",Projects[[  ]]*175)</f>
+        <v/>
+      </c>
+      <c r="G20" s="17">
+        <f t="array" ref="G20">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
+        <v>0</v>
+      </c>
+      <c r="H20" s="2"/>
+    </row>
+    <row r="21" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="B21" s="29"/>
+      <c r="C21" s="18">
         <v>42888</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="21">
-        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
-        <v>1E-4</v>
-      </c>
-      <c r="E21" s="20" t="str">
-        <f>REPT("|",Projects[[  ]]*175)</f>
-        <v/>
-      </c>
-      <c r="F21" s="17">
-        <f t="array" ref="F21">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
-        <v>0</v>
-      </c>
-      <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="22">
+      <c r="D21" s="2"/>
+      <c r="E21" s="21">
+        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
+        <v>1E-4</v>
+      </c>
+      <c r="F21" s="20" t="str">
+        <f>REPT("|",Projects[[  ]]*175)</f>
+        <v/>
+      </c>
+      <c r="G21" s="17">
+        <f t="array" ref="G21">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
+        <v>0</v>
+      </c>
+      <c r="H21" s="2"/>
+    </row>
+    <row r="22" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B22" s="29"/>
+      <c r="C22" s="22">
         <v>42889</v>
       </c>
-      <c r="C22" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="D22" s="21">
-        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
-        <v>1E-4</v>
-      </c>
-      <c r="E22" s="20" t="str">
-        <f>REPT("|",Projects[[  ]]*175)</f>
-        <v/>
-      </c>
-      <c r="F22" s="17">
-        <f t="array" ref="F22">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
-        <v>0</v>
-      </c>
-      <c r="G22" s="27"/>
-    </row>
-    <row r="23" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="22">
+      <c r="D22" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" s="21">
+        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
+        <v>1E-4</v>
+      </c>
+      <c r="F22" s="20" t="str">
+        <f>REPT("|",Projects[[  ]]*175)</f>
+        <v/>
+      </c>
+      <c r="G22" s="17">
+        <f t="array" ref="G22">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
+        <v>0</v>
+      </c>
+      <c r="H22" s="27"/>
+    </row>
+    <row r="23" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="B23" s="29"/>
+      <c r="C23" s="22">
         <v>42890</v>
       </c>
-      <c r="C23" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="D23" s="21">
-        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
-        <v>1E-4</v>
-      </c>
-      <c r="E23" s="20" t="str">
-        <f>REPT("|",Projects[[  ]]*175)</f>
-        <v/>
-      </c>
-      <c r="F23" s="17">
-        <f t="array" ref="F23">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
-        <v>0</v>
-      </c>
-      <c r="G23" s="27"/>
-    </row>
-    <row r="24" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="22">
+      <c r="D23" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="E23" s="21">
+        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
+        <v>1E-4</v>
+      </c>
+      <c r="F23" s="20" t="str">
+        <f>REPT("|",Projects[[  ]]*175)</f>
+        <v/>
+      </c>
+      <c r="G23" s="17">
+        <f t="array" ref="G23">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
+        <v>0</v>
+      </c>
+      <c r="H23" s="27"/>
+    </row>
+    <row r="24" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" s="29"/>
+      <c r="C24" s="22">
         <v>42891</v>
       </c>
-      <c r="C24" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="D24" s="21">
-        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
-        <v>1E-4</v>
-      </c>
-      <c r="E24" s="20" t="str">
-        <f>REPT("|",Projects[[  ]]*175)</f>
-        <v/>
-      </c>
-      <c r="F24" s="17">
-        <f t="array" ref="F24">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
-        <v>0</v>
-      </c>
-      <c r="G24" s="27"/>
-    </row>
-    <row r="25" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="18">
+      <c r="D24" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24" s="21">
+        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
+        <v>1E-4</v>
+      </c>
+      <c r="F24" s="20" t="str">
+        <f>REPT("|",Projects[[  ]]*175)</f>
+        <v/>
+      </c>
+      <c r="G24" s="17">
+        <f t="array" ref="G24">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
+        <v>0</v>
+      </c>
+      <c r="H24" s="27"/>
+    </row>
+    <row r="25" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B25" s="29"/>
+      <c r="C25" s="18">
         <v>42892</v>
       </c>
-      <c r="C25" s="2"/>
-      <c r="D25" s="21">
-        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
-        <v>1E-4</v>
-      </c>
-      <c r="E25" s="20" t="str">
-        <f>REPT("|",Projects[[  ]]*175)</f>
-        <v/>
-      </c>
-      <c r="F25" s="17">
-        <f t="array" ref="F25">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
-        <v>0</v>
-      </c>
-      <c r="G25" s="2"/>
-    </row>
-    <row r="26" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="18">
+      <c r="D25" s="2"/>
+      <c r="E25" s="21">
+        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
+        <v>1E-4</v>
+      </c>
+      <c r="F25" s="20" t="str">
+        <f>REPT("|",Projects[[  ]]*175)</f>
+        <v/>
+      </c>
+      <c r="G25" s="17">
+        <f t="array" ref="G25">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
+        <v>0</v>
+      </c>
+      <c r="H25" s="2"/>
+    </row>
+    <row r="26" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" s="29"/>
+      <c r="C26" s="18">
         <v>42893</v>
       </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="21">
-        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
-        <v>1E-4</v>
-      </c>
-      <c r="E26" s="20" t="str">
-        <f>REPT("|",Projects[[  ]]*175)</f>
-        <v/>
-      </c>
-      <c r="F26" s="17">
-        <f t="array" ref="F26">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
-        <v>0</v>
-      </c>
-      <c r="G26" s="2"/>
-    </row>
-    <row r="27" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="18">
+      <c r="D26" s="2"/>
+      <c r="E26" s="21">
+        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
+        <v>1E-4</v>
+      </c>
+      <c r="F26" s="20" t="str">
+        <f>REPT("|",Projects[[  ]]*175)</f>
+        <v/>
+      </c>
+      <c r="G26" s="17">
+        <f t="array" ref="G26">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
+        <v>0</v>
+      </c>
+      <c r="H26" s="2"/>
+    </row>
+    <row r="27" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" s="29"/>
+      <c r="C27" s="18">
         <v>42894</v>
       </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="21">
-        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
-        <v>1E-4</v>
-      </c>
-      <c r="E27" s="20" t="str">
-        <f>REPT("|",Projects[[  ]]*175)</f>
-        <v/>
-      </c>
-      <c r="F27" s="17">
-        <f t="array" ref="F27">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
-        <v>0</v>
-      </c>
-      <c r="G27" s="2"/>
-    </row>
-    <row r="28" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="18">
+      <c r="D27" s="2"/>
+      <c r="E27" s="21">
+        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
+        <v>1E-4</v>
+      </c>
+      <c r="F27" s="20" t="str">
+        <f>REPT("|",Projects[[  ]]*175)</f>
+        <v/>
+      </c>
+      <c r="G27" s="17">
+        <f t="array" ref="G27">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
+        <v>0</v>
+      </c>
+      <c r="H27" s="2"/>
+    </row>
+    <row r="28" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" s="29"/>
+      <c r="C28" s="18">
         <v>42895</v>
       </c>
-      <c r="C28" s="2"/>
-      <c r="D28" s="21">
-        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
-        <v>1E-4</v>
-      </c>
-      <c r="E28" s="20" t="str">
-        <f>REPT("|",Projects[[  ]]*175)</f>
-        <v/>
-      </c>
-      <c r="F28" s="17">
-        <f t="array" ref="F28">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
-        <v>0</v>
-      </c>
-      <c r="G28" s="2"/>
-    </row>
-    <row r="29" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="18">
+      <c r="D28" s="2"/>
+      <c r="E28" s="21">
+        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
+        <v>1E-4</v>
+      </c>
+      <c r="F28" s="20" t="str">
+        <f>REPT("|",Projects[[  ]]*175)</f>
+        <v/>
+      </c>
+      <c r="G28" s="17">
+        <f t="array" ref="G28">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
+        <v>0</v>
+      </c>
+      <c r="H28" s="2"/>
+    </row>
+    <row r="29" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B29" s="29"/>
+      <c r="C29" s="22">
         <v>42896</v>
       </c>
-      <c r="C29" s="2"/>
-      <c r="D29" s="21">
-        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
-        <v>1E-4</v>
-      </c>
-      <c r="E29" s="20" t="str">
-        <f>REPT("|",Projects[[  ]]*175)</f>
-        <v/>
-      </c>
-      <c r="F29" s="17">
-        <f t="array" ref="F29">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
-        <v>0</v>
-      </c>
-      <c r="G29" s="2"/>
-    </row>
-    <row r="30" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="22">
+      <c r="D29" s="27"/>
+      <c r="E29" s="21">
+        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
+        <v>1E-4</v>
+      </c>
+      <c r="F29" s="20" t="str">
+        <f>REPT("|",Projects[[  ]]*175)</f>
+        <v/>
+      </c>
+      <c r="G29" s="17">
+        <f t="array" ref="G29">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
+        <v>0</v>
+      </c>
+      <c r="H29" s="27"/>
+    </row>
+    <row r="30" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="B30" s="29"/>
+      <c r="C30" s="22">
         <v>42897</v>
       </c>
-      <c r="C30" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="D30" s="21">
-        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
-        <v>1E-4</v>
-      </c>
-      <c r="E30" s="20" t="str">
-        <f>REPT("|",Projects[[  ]]*175)</f>
-        <v/>
-      </c>
-      <c r="F30" s="17">
-        <f t="array" ref="F30">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
-        <v>0</v>
-      </c>
-      <c r="G30" s="27"/>
-    </row>
-    <row r="31" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="22">
+      <c r="D30" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="E30" s="21">
+        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
+        <v>1E-4</v>
+      </c>
+      <c r="F30" s="20" t="str">
+        <f>REPT("|",Projects[[  ]]*175)</f>
+        <v/>
+      </c>
+      <c r="G30" s="17">
+        <f t="array" ref="G30">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
+        <v>0</v>
+      </c>
+      <c r="H30" s="27"/>
+    </row>
+    <row r="31" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" s="29"/>
+      <c r="C31" s="18">
         <v>42898</v>
       </c>
-      <c r="C31" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="D31" s="21">
-        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
-        <v>1E-4</v>
-      </c>
-      <c r="E31" s="20" t="str">
-        <f>REPT("|",Projects[[  ]]*175)</f>
-        <v/>
-      </c>
-      <c r="F31" s="17">
-        <f t="array" ref="F31">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
-        <v>0</v>
-      </c>
-      <c r="G31" s="27"/>
-    </row>
-    <row r="32" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="18">
+      <c r="E31" s="21">
+        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
+        <v>1E-4</v>
+      </c>
+      <c r="F31" s="20" t="str">
+        <f>REPT("|",Projects[[  ]]*175)</f>
+        <v/>
+      </c>
+      <c r="G31" s="17">
+        <f t="array" ref="G31">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B32" s="29"/>
+      <c r="C32" s="18">
         <v>42899</v>
       </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="19">
-        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
-        <v>1E-4</v>
-      </c>
-      <c r="E32" s="20" t="str">
-        <f>REPT("|",Projects[[  ]]*175)</f>
-        <v/>
-      </c>
-      <c r="F32" s="17">
-        <f t="array" ref="F32">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
-        <v>0</v>
-      </c>
-      <c r="G32" s="2"/>
-    </row>
-    <row r="33" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="18">
+      <c r="D32" s="2"/>
+      <c r="E32" s="19">
+        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
+        <v>1E-4</v>
+      </c>
+      <c r="F32" s="20" t="str">
+        <f>REPT("|",Projects[[  ]]*175)</f>
+        <v/>
+      </c>
+      <c r="G32" s="17">
+        <f t="array" ref="G32">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
+        <v>0</v>
+      </c>
+      <c r="H32" s="2"/>
+    </row>
+    <row r="33" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="B33" s="29"/>
+      <c r="C33" s="18">
         <v>42900</v>
       </c>
-      <c r="C33" s="2"/>
-      <c r="D33" s="19">
-        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
-        <v>1E-4</v>
-      </c>
-      <c r="E33" s="20" t="str">
-        <f>REPT("|",Projects[[  ]]*175)</f>
-        <v/>
-      </c>
-      <c r="F33" s="17">
-        <f t="array" ref="F33">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
-        <v>0</v>
-      </c>
-      <c r="G33" s="2"/>
-    </row>
-    <row r="34" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="18">
+      <c r="D33" s="2"/>
+      <c r="E33" s="19">
+        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
+        <v>1E-4</v>
+      </c>
+      <c r="F33" s="20" t="str">
+        <f>REPT("|",Projects[[  ]]*175)</f>
+        <v/>
+      </c>
+      <c r="G33" s="17">
+        <f t="array" ref="G33">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
+        <v>0</v>
+      </c>
+      <c r="H33" s="2"/>
+    </row>
+    <row r="34" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B34" s="29"/>
+      <c r="C34" s="18">
         <v>42901</v>
       </c>
-      <c r="C34" s="2"/>
-      <c r="D34" s="19">
-        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
-        <v>1E-4</v>
-      </c>
-      <c r="E34" s="20" t="str">
-        <f>REPT("|",Projects[[  ]]*175)</f>
-        <v/>
-      </c>
-      <c r="F34" s="17">
-        <f t="array" ref="F34">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
-        <v>0</v>
-      </c>
-      <c r="G34" s="2"/>
-    </row>
-    <row r="35" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="18">
+      <c r="D34" s="2"/>
+      <c r="E34" s="19">
+        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
+        <v>1E-4</v>
+      </c>
+      <c r="F34" s="20" t="str">
+        <f>REPT("|",Projects[[  ]]*175)</f>
+        <v/>
+      </c>
+      <c r="G34" s="17">
+        <f t="array" ref="G34">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
+        <v>0</v>
+      </c>
+      <c r="H34" s="2"/>
+    </row>
+    <row r="35" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="B35" s="29"/>
+      <c r="C35" s="18">
         <v>42902</v>
       </c>
-      <c r="C35" s="2"/>
-      <c r="D35" s="19">
-        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
-        <v>1E-4</v>
-      </c>
-      <c r="E35" s="20" t="str">
-        <f>REPT("|",Projects[[  ]]*175)</f>
-        <v/>
-      </c>
-      <c r="F35" s="17">
-        <f t="array" ref="F35">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
-        <v>0</v>
-      </c>
-      <c r="G35" s="2"/>
-    </row>
-    <row r="36" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="18">
+      <c r="D35" s="2"/>
+      <c r="E35" s="19">
+        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
+        <v>1E-4</v>
+      </c>
+      <c r="F35" s="20" t="str">
+        <f>REPT("|",Projects[[  ]]*175)</f>
+        <v/>
+      </c>
+      <c r="G35" s="17">
+        <f t="array" ref="G35">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
+        <v>0</v>
+      </c>
+      <c r="H35" s="2"/>
+    </row>
+    <row r="36" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B36" s="29"/>
+      <c r="C36" s="18">
         <v>42903</v>
       </c>
-      <c r="C36" s="2"/>
-      <c r="D36" s="19">
-        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
-        <v>1E-4</v>
-      </c>
-      <c r="E36" s="20" t="str">
-        <f>REPT("|",Projects[[  ]]*175)</f>
-        <v/>
-      </c>
-      <c r="F36" s="17">
-        <f t="array" ref="F36">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
-        <v>0</v>
-      </c>
-      <c r="G36" s="2"/>
-    </row>
-    <row r="37" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="22">
+      <c r="D36" s="2"/>
+      <c r="E36" s="19">
+        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
+        <v>1E-4</v>
+      </c>
+      <c r="F36" s="20" t="str">
+        <f>REPT("|",Projects[[  ]]*175)</f>
+        <v/>
+      </c>
+      <c r="G36" s="17">
+        <f t="array" ref="G36">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
+        <v>0</v>
+      </c>
+      <c r="H36" s="2"/>
+    </row>
+    <row r="37" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="B37" s="29"/>
+      <c r="C37" s="22">
         <v>42904</v>
       </c>
-      <c r="C37" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="D37" s="19">
-        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
-        <v>1E-4</v>
-      </c>
-      <c r="E37" s="20" t="str">
-        <f>REPT("|",Projects[[  ]]*175)</f>
-        <v/>
-      </c>
-      <c r="F37" s="17">
-        <f t="array" ref="F37">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
-        <v>0</v>
-      </c>
-      <c r="G37" s="27"/>
-    </row>
-    <row r="38" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="22">
+      <c r="D37" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="E37" s="19">
+        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
+        <v>1E-4</v>
+      </c>
+      <c r="F37" s="20" t="str">
+        <f>REPT("|",Projects[[  ]]*175)</f>
+        <v/>
+      </c>
+      <c r="G37" s="17">
+        <f t="array" ref="G37">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
+        <v>0</v>
+      </c>
+      <c r="H37" s="27"/>
+    </row>
+    <row r="38" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="B38" s="29"/>
+      <c r="C38" s="22">
         <v>42905</v>
       </c>
-      <c r="C38" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="D38" s="19">
-        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
-        <v>1E-4</v>
-      </c>
-      <c r="E38" s="20" t="str">
-        <f>REPT("|",Projects[[  ]]*175)</f>
-        <v/>
-      </c>
-      <c r="F38" s="17">
-        <f t="array" ref="F38">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
-        <v>0</v>
-      </c>
-      <c r="G38" s="27"/>
-    </row>
-    <row r="39" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="18">
+      <c r="D38" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="E38" s="19">
+        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
+        <v>1E-4</v>
+      </c>
+      <c r="F38" s="20" t="str">
+        <f>REPT("|",Projects[[  ]]*175)</f>
+        <v/>
+      </c>
+      <c r="G38" s="17">
+        <f t="array" ref="G38">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
+        <v>0</v>
+      </c>
+      <c r="H38" s="27"/>
+    </row>
+    <row r="39" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B39" s="29"/>
+      <c r="C39" s="18">
         <v>42906</v>
       </c>
-      <c r="C39" s="2"/>
-      <c r="D39" s="19">
-        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
-        <v>1E-4</v>
-      </c>
-      <c r="E39" s="20" t="str">
-        <f>REPT("|",Projects[[  ]]*175)</f>
-        <v/>
-      </c>
-      <c r="F39" s="17">
-        <f t="array" ref="F39">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
-        <v>0</v>
-      </c>
-      <c r="G39" s="2"/>
-    </row>
-    <row r="40" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="18">
+      <c r="D39" s="2"/>
+      <c r="E39" s="19">
+        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
+        <v>1E-4</v>
+      </c>
+      <c r="F39" s="20" t="str">
+        <f>REPT("|",Projects[[  ]]*175)</f>
+        <v/>
+      </c>
+      <c r="G39" s="17">
+        <f t="array" ref="G39">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
+        <v>0</v>
+      </c>
+      <c r="H39" s="2"/>
+    </row>
+    <row r="40" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="B40" s="29"/>
+      <c r="C40" s="18">
         <v>42907</v>
       </c>
-      <c r="C40" s="2"/>
-      <c r="D40" s="19">
-        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
-        <v>1E-4</v>
-      </c>
-      <c r="E40" s="20" t="str">
-        <f>REPT("|",Projects[[  ]]*175)</f>
-        <v/>
-      </c>
-      <c r="F40" s="17">
-        <f t="array" ref="F40">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
-        <v>0</v>
-      </c>
-      <c r="G40" s="2"/>
-    </row>
-    <row r="41" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="18">
+      <c r="D40" s="2"/>
+      <c r="E40" s="19">
+        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
+        <v>1E-4</v>
+      </c>
+      <c r="F40" s="20" t="str">
+        <f>REPT("|",Projects[[  ]]*175)</f>
+        <v/>
+      </c>
+      <c r="G40" s="17">
+        <f t="array" ref="G40">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
+        <v>0</v>
+      </c>
+      <c r="H40" s="2"/>
+    </row>
+    <row r="41" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="B41" s="29"/>
+      <c r="C41" s="18">
         <v>42908</v>
       </c>
-      <c r="C41" s="2"/>
-      <c r="D41" s="19">
-        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
-        <v>1E-4</v>
-      </c>
-      <c r="E41" s="20" t="str">
-        <f>REPT("|",Projects[[  ]]*175)</f>
-        <v/>
-      </c>
-      <c r="F41" s="17">
-        <f t="array" ref="F41">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
-        <v>0</v>
-      </c>
-      <c r="G41" s="2"/>
-    </row>
-    <row r="42" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="18">
+      <c r="D41" s="2"/>
+      <c r="E41" s="19">
+        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
+        <v>1E-4</v>
+      </c>
+      <c r="F41" s="20" t="str">
+        <f>REPT("|",Projects[[  ]]*175)</f>
+        <v/>
+      </c>
+      <c r="G41" s="17">
+        <f t="array" ref="G41">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
+        <v>0</v>
+      </c>
+      <c r="H41" s="2"/>
+    </row>
+    <row r="42" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="B42" s="29"/>
+      <c r="C42" s="18">
         <v>42909</v>
       </c>
-      <c r="C42" s="2"/>
-      <c r="D42" s="19">
-        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
-        <v>1E-4</v>
-      </c>
-      <c r="E42" s="20" t="str">
-        <f>REPT("|",Projects[[  ]]*175)</f>
-        <v/>
-      </c>
-      <c r="F42" s="17">
-        <f t="array" ref="F42">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
-        <v>0</v>
-      </c>
-      <c r="G42" s="2"/>
-    </row>
-    <row r="43" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="18">
+      <c r="D42" s="2"/>
+      <c r="E42" s="19">
+        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
+        <v>1E-4</v>
+      </c>
+      <c r="F42" s="20" t="str">
+        <f>REPT("|",Projects[[  ]]*175)</f>
+        <v/>
+      </c>
+      <c r="G42" s="17">
+        <f t="array" ref="G42">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
+        <v>0</v>
+      </c>
+      <c r="H42" s="2"/>
+    </row>
+    <row r="43" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="29" t="s">
+        <v>64</v>
+      </c>
+      <c r="B43" s="29"/>
+      <c r="C43" s="18">
         <v>42910</v>
       </c>
-      <c r="C43" s="2"/>
-      <c r="D43" s="19">
-        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
-        <v>1E-4</v>
-      </c>
-      <c r="E43" s="20" t="str">
-        <f>REPT("|",Projects[[  ]]*175)</f>
-        <v/>
-      </c>
-      <c r="F43" s="17">
-        <f t="array" ref="F43">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
-        <v>0</v>
-      </c>
-      <c r="G43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="19">
+        <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
+        <v>1E-4</v>
+      </c>
+      <c r="F43" s="20" t="str">
+        <f>REPT("|",Projects[[  ]]*175)</f>
+        <v/>
+      </c>
+      <c r="G43" s="17">
+        <f t="array" ref="G43">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
+        <v>0</v>
+      </c>
+      <c r="H43" s="2"/>
+    </row>
+    <row r="44" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="29"/>
+      <c r="B44" s="29"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>

</xml_diff>

<commit_message>
fixed login and changed everthing to PHP
</commit_message>
<xml_diff>
--- a/documents/@Planner/Planner biocodegaming.xlsx
+++ b/documents/@Planner/Planner biocodegaming.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="71">
   <si>
     <t>Project</t>
   </si>
@@ -276,6 +276,12 @@
   </si>
   <si>
     <t>het uurt te lang ugh</t>
+  </si>
+  <si>
+    <t>alex heeft een basic forum en damian is met de login en reg bezig</t>
+  </si>
+  <si>
+    <t xml:space="preserve">forum wordt ge implementeerd </t>
   </si>
 </sst>
 </file>
@@ -2189,12 +2195,13 @@
   </sheetPr>
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView showGridLines="0" showZeros="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="11" customWidth="1"/>
     <col min="2" max="2" width="3.875" customWidth="1"/>
     <col min="3" max="3" width="34.25" customWidth="1"/>
     <col min="4" max="4" width="71" customWidth="1"/>
@@ -2581,10 +2588,12 @@
         <v>59</v>
       </c>
       <c r="B17" s="29"/>
-      <c r="C17" s="18">
+      <c r="C17" s="26">
         <v>42884</v>
       </c>
-      <c r="D17" s="2"/>
+      <c r="D17" s="2" t="s">
+        <v>69</v>
+      </c>
       <c r="E17" s="21">
         <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
         <v>1E-4</v>
@@ -2597,7 +2606,9 @@
         <f t="array" ref="G17">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
         <v>0</v>
       </c>
-      <c r="H17" s="2"/>
+      <c r="H17" s="2" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="18" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="29" t="s">

</xml_diff>

<commit_message>
fixed error with SESSION
</commit_message>
<xml_diff>
--- a/documents/@Planner/Planner biocodegaming.xlsx
+++ b/documents/@Planner/Planner biocodegaming.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="74">
   <si>
     <t>Project</t>
   </si>
@@ -285,6 +285,12 @@
   </si>
   <si>
     <t>alex werkt verder met de forum en damian werkt enkele musts af</t>
+  </si>
+  <si>
+    <t>alex heeft logout gefinished</t>
+  </si>
+  <si>
+    <t>damian was ziek</t>
   </si>
 </sst>
 </file>
@@ -2198,8 +2204,8 @@
   </sheetPr>
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView showGridLines="0" showZeros="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2668,7 +2674,7 @@
         <v>62</v>
       </c>
       <c r="B20" s="29"/>
-      <c r="C20" s="18">
+      <c r="C20" s="26">
         <v>42887</v>
       </c>
       <c r="D20" s="2"/>
@@ -2691,10 +2697,12 @@
         <v>63</v>
       </c>
       <c r="B21" s="29"/>
-      <c r="C21" s="18">
+      <c r="C21" s="26">
         <v>42888</v>
       </c>
-      <c r="D21" s="2"/>
+      <c r="D21" s="2" t="s">
+        <v>72</v>
+      </c>
       <c r="E21" s="21">
         <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
         <v>1E-4</v>
@@ -2707,7 +2715,9 @@
         <f t="array" ref="G21">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
         <v>0</v>
       </c>
-      <c r="H21" s="2"/>
+      <c r="H21" s="2" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="22" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="29" t="s">

</xml_diff>

<commit_message>
Revert "finish some little things"
This reverts commit 5f7202161cbcd88c42abd4ccd1d0609501ca6759.
</commit_message>
<xml_diff>
--- a/documents/@Planner/Planner biocodegaming.xlsx
+++ b/documents/@Planner/Planner biocodegaming.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="74">
   <si>
     <t>Project</t>
   </si>
@@ -291,15 +291,6 @@
   </si>
   <si>
     <t>damian was ziek</t>
-  </si>
-  <si>
-    <t>poster begin en indeling voor filmpje</t>
-  </si>
-  <si>
-    <t>alex leert een pm system te maken en damian heeft user info page af</t>
-  </si>
-  <si>
-    <t>alex is bezig met inventory en damian werkt aan posters</t>
   </si>
 </sst>
 </file>
@@ -2213,8 +2204,8 @@
   </sheetPr>
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView showGridLines="0" showZeros="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2808,12 +2799,10 @@
         <v>60</v>
       </c>
       <c r="B25" s="29"/>
-      <c r="C25" s="26">
+      <c r="C25" s="18">
         <v>42892</v>
       </c>
-      <c r="D25" s="2" t="s">
-        <v>75</v>
-      </c>
+      <c r="D25" s="2"/>
       <c r="E25" s="21">
         <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
         <v>1E-4</v>
@@ -2833,12 +2822,10 @@
         <v>61</v>
       </c>
       <c r="B26" s="29"/>
-      <c r="C26" s="26">
+      <c r="C26" s="18">
         <v>42893</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>76</v>
-      </c>
+      <c r="D26" s="2"/>
       <c r="E26" s="21">
         <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
         <v>1E-4</v>
@@ -2858,12 +2845,10 @@
         <v>62</v>
       </c>
       <c r="B27" s="29"/>
-      <c r="C27" s="26">
+      <c r="C27" s="18">
         <v>42894</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>51</v>
-      </c>
+      <c r="D27" s="2"/>
       <c r="E27" s="21">
         <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
         <v>1E-4</v>
@@ -2883,12 +2868,10 @@
         <v>63</v>
       </c>
       <c r="B28" s="29"/>
-      <c r="C28" s="26">
+      <c r="C28" s="18">
         <v>42895</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>74</v>
-      </c>
+      <c r="D28" s="2"/>
       <c r="E28" s="21">
         <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
         <v>1E-4</v>

</xml_diff>

<commit_message>
finish some little things
</commit_message>
<xml_diff>
--- a/documents/@Planner/Planner biocodegaming.xlsx
+++ b/documents/@Planner/Planner biocodegaming.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="77">
   <si>
     <t>Project</t>
   </si>
@@ -291,6 +291,15 @@
   </si>
   <si>
     <t>damian was ziek</t>
+  </si>
+  <si>
+    <t>poster begin en indeling voor filmpje</t>
+  </si>
+  <si>
+    <t>alex leert een pm system te maken en damian heeft user info page af</t>
+  </si>
+  <si>
+    <t>alex is bezig met inventory en damian werkt aan posters</t>
   </si>
 </sst>
 </file>
@@ -2204,8 +2213,8 @@
   </sheetPr>
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView showGridLines="0" showZeros="0" tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2799,10 +2808,12 @@
         <v>60</v>
       </c>
       <c r="B25" s="29"/>
-      <c r="C25" s="18">
+      <c r="C25" s="26">
         <v>42892</v>
       </c>
-      <c r="D25" s="2"/>
+      <c r="D25" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="E25" s="21">
         <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
         <v>1E-4</v>
@@ -2822,10 +2833,12 @@
         <v>61</v>
       </c>
       <c r="B26" s="29"/>
-      <c r="C26" s="18">
+      <c r="C26" s="26">
         <v>42893</v>
       </c>
-      <c r="D26" s="2"/>
+      <c r="D26" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="E26" s="21">
         <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
         <v>1E-4</v>
@@ -2845,10 +2858,12 @@
         <v>62</v>
       </c>
       <c r="B27" s="29"/>
-      <c r="C27" s="18">
+      <c r="C27" s="26">
         <v>42894</v>
       </c>
-      <c r="D27" s="2"/>
+      <c r="D27" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="E27" s="21">
         <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
         <v>1E-4</v>
@@ -2868,10 +2883,12 @@
         <v>63</v>
       </c>
       <c r="B28" s="29"/>
-      <c r="C28" s="18">
+      <c r="C28" s="26">
         <v>42895</v>
       </c>
-      <c r="D28" s="2"/>
+      <c r="D28" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="E28" s="21">
         <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
         <v>1E-4</v>

</xml_diff>

<commit_message>
Revert "Revert "finish some little things""
This reverts commit 51becea9e1c5248b47a26ba55afd71822453d943.
</commit_message>
<xml_diff>
--- a/documents/@Planner/Planner biocodegaming.xlsx
+++ b/documents/@Planner/Planner biocodegaming.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="77">
   <si>
     <t>Project</t>
   </si>
@@ -291,6 +291,15 @@
   </si>
   <si>
     <t>damian was ziek</t>
+  </si>
+  <si>
+    <t>poster begin en indeling voor filmpje</t>
+  </si>
+  <si>
+    <t>alex leert een pm system te maken en damian heeft user info page af</t>
+  </si>
+  <si>
+    <t>alex is bezig met inventory en damian werkt aan posters</t>
   </si>
 </sst>
 </file>
@@ -2204,8 +2213,8 @@
   </sheetPr>
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView showGridLines="0" showZeros="0" tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2799,10 +2808,12 @@
         <v>60</v>
       </c>
       <c r="B25" s="29"/>
-      <c r="C25" s="18">
+      <c r="C25" s="26">
         <v>42892</v>
       </c>
-      <c r="D25" s="2"/>
+      <c r="D25" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="E25" s="21">
         <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
         <v>1E-4</v>
@@ -2822,10 +2833,12 @@
         <v>61</v>
       </c>
       <c r="B26" s="29"/>
-      <c r="C26" s="18">
+      <c r="C26" s="26">
         <v>42893</v>
       </c>
-      <c r="D26" s="2"/>
+      <c r="D26" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="E26" s="21">
         <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
         <v>1E-4</v>
@@ -2845,10 +2858,12 @@
         <v>62</v>
       </c>
       <c r="B27" s="29"/>
-      <c r="C27" s="18">
+      <c r="C27" s="26">
         <v>42894</v>
       </c>
-      <c r="D27" s="2"/>
+      <c r="D27" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="E27" s="21">
         <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
         <v>1E-4</v>
@@ -2868,10 +2883,12 @@
         <v>63</v>
       </c>
       <c r="B28" s="29"/>
-      <c r="C28" s="18">
+      <c r="C28" s="26">
         <v>42895</v>
       </c>
-      <c r="D28" s="2"/>
+      <c r="D28" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="E28" s="21">
         <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
         <v>1E-4</v>

</xml_diff>

<commit_message>
one giant update whoohooooo
</commit_message>
<xml_diff>
--- a/documents/@Planner/Planner biocodegaming.xlsx
+++ b/documents/@Planner/Planner biocodegaming.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="80">
   <si>
     <t>Project</t>
   </si>
@@ -300,6 +300,15 @@
   </si>
   <si>
     <t>alex is bezig met inventory en damian werkt aan posters</t>
+  </si>
+  <si>
+    <t>damian heeft poster's gemaakt en alex maakt de app</t>
+  </si>
+  <si>
+    <t>damian heeft adjustments gemaakt aan de posters en alex werkt aan de app</t>
+  </si>
+  <si>
+    <t>alex werkt og aan de app en damian maakt user inventory</t>
   </si>
 </sst>
 </file>
@@ -2213,8 +2222,8 @@
   </sheetPr>
   <dimension ref="A1:H44"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+    <sheetView showGridLines="0" showZeros="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2956,8 +2965,11 @@
         <v>59</v>
       </c>
       <c r="B31" s="29"/>
-      <c r="C31" s="18">
+      <c r="C31" s="26">
         <v>42898</v>
+      </c>
+      <c r="D31" t="s">
+        <v>77</v>
       </c>
       <c r="E31" s="21">
         <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
@@ -2977,10 +2989,12 @@
         <v>60</v>
       </c>
       <c r="B32" s="29"/>
-      <c r="C32" s="18">
+      <c r="C32" s="26">
         <v>42899</v>
       </c>
-      <c r="D32" s="2"/>
+      <c r="D32" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="E32" s="19">
         <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
         <v>1E-4</v>
@@ -3000,10 +3014,12 @@
         <v>61</v>
       </c>
       <c r="B33" s="29"/>
-      <c r="C33" s="18">
+      <c r="C33" s="26">
         <v>42900</v>
       </c>
-      <c r="D33" s="2"/>
+      <c r="D33" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="E33" s="19">
         <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
         <v>1E-4</v>
@@ -3023,10 +3039,12 @@
         <v>62</v>
       </c>
       <c r="B34" s="29"/>
-      <c r="C34" s="18">
+      <c r="C34" s="26">
         <v>42901</v>
       </c>
-      <c r="D34" s="2"/>
+      <c r="D34" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="E34" s="19">
         <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
         <v>1E-4</v>
@@ -3069,10 +3087,12 @@
         <v>64</v>
       </c>
       <c r="B36" s="29"/>
-      <c r="C36" s="18">
+      <c r="C36" s="22">
         <v>42903</v>
       </c>
-      <c r="D36" s="2"/>
+      <c r="D36" s="27" t="s">
+        <v>49</v>
+      </c>
       <c r="E36" s="19">
         <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
         <v>1E-4</v>
@@ -3085,7 +3105,7 @@
         <f t="array" ref="G36">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
         <v>0</v>
       </c>
-      <c r="H36" s="2"/>
+      <c r="H36" s="27"/>
     </row>
     <row r="37" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="29" t="s">
@@ -3117,11 +3137,8 @@
         <v>59</v>
       </c>
       <c r="B38" s="29"/>
-      <c r="C38" s="22">
+      <c r="C38" s="18">
         <v>42905</v>
-      </c>
-      <c r="D38" s="27" t="s">
-        <v>49</v>
       </c>
       <c r="E38" s="19">
         <f>IFERROR((SUMIFS(Tasks[Done],Tasks[Project],Projects[[#This Row],[Project]])/COUNTIFS(Tasks[Project],Projects[[#This Row],[Project]]))+0.0001,0.0001)</f>
@@ -3135,7 +3152,6 @@
         <f t="array" ref="G38">MAX(IF((Tasks[Project]=Projects[[#This Row],[Project]])*(Tasks[Start]&gt;0),Tasks[[Start]:[End]]))</f>
         <v>0</v>
       </c>
-      <c r="H38" s="27"/>
     </row>
     <row r="39" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="29" t="s">

</xml_diff>